<commit_message>
50 texts per dataset in ARTS
</commit_message>
<xml_diff>
--- a/workspace/datasets/__clustering_of_LFs/manualLF2C.xlsx
+++ b/workspace/datasets/__clustering_of_LFs/manualLF2C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christin/Desktop/USB-Pipeline/workspace/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christin/Desktop/USB-Pipeline/workspace/datasets/__clustering_of_LFs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B15459-F5B9-3F4C-899D-D2F9DC267B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C674E98A-2A80-5E4E-9669-93799C50ABBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11080" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{B53BDDDE-F7CE-7D4E-8D36-81EE01EDCD84}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{B53BDDDE-F7CE-7D4E-8D36-81EE01EDCD84}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="341">
   <si>
     <t>clustered</t>
   </si>
@@ -1053,6 +1053,12 @@
   </si>
   <si>
     <t>no_relative_sub_clauses_label=NOT_SIMPLE_thresh={thresh}</t>
+  </si>
+  <si>
+    <t>low_relative_sub_clauses_ratio_label=NOT_SIMPLE_thresh={thresh}</t>
+  </si>
+  <si>
+    <t>low_relative_sub_clauses_ratio_label=SIMPLE_thresh={thresh}</t>
   </si>
 </sst>
 </file>
@@ -1088,8 +1094,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1406,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DCE332-C261-6947-BE11-E959C673661A}">
   <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2198,7 +2205,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B47" t="s">
@@ -2215,8 +2222,8 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>131</v>
+      <c r="A48" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="B48" t="s">
         <v>38</v>
@@ -2228,46 +2235,40 @@
         <v>133</v>
       </c>
       <c r="E48" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="D49" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E49" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C50" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="D50" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E50" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
         <v>63</v>
@@ -2276,12 +2277,12 @@
         <v>138</v>
       </c>
       <c r="E51" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B52" t="s">
         <v>63</v>
@@ -2290,74 +2291,80 @@
         <v>138</v>
       </c>
       <c r="E52" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
         <v>63</v>
       </c>
+      <c r="C53" t="s">
+        <v>147</v>
+      </c>
       <c r="D53" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="E53" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
         <v>63</v>
       </c>
+      <c r="C54" t="s">
+        <v>147</v>
+      </c>
       <c r="D54" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="E54" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B55" t="s">
         <v>63</v>
       </c>
       <c r="C55" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D55" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E55" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B56" t="s">
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D56" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E56" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B57" t="s">
         <v>63</v>
@@ -2369,12 +2376,12 @@
         <v>154</v>
       </c>
       <c r="E57" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B58" t="s">
         <v>63</v>
@@ -2386,46 +2393,46 @@
         <v>154</v>
       </c>
       <c r="E58" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>153</v>
+        <v>27</v>
       </c>
       <c r="D59" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E59" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>153</v>
+        <v>27</v>
       </c>
       <c r="D60" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E60" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B61" t="s">
         <v>6</v>
@@ -2434,15 +2441,15 @@
         <v>27</v>
       </c>
       <c r="D61" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E61" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B62" t="s">
         <v>6</v>
@@ -2451,49 +2458,49 @@
         <v>27</v>
       </c>
       <c r="D62" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E62" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B63" t="s">
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>173</v>
       </c>
       <c r="D63" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="E63" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>173</v>
       </c>
       <c r="D64" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="E64" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B65" t="s">
         <v>6</v>
@@ -2505,12 +2512,12 @@
         <v>174</v>
       </c>
       <c r="E65" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>176</v>
+        <v>335</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
@@ -2522,182 +2529,182 @@
         <v>174</v>
       </c>
       <c r="E66" t="s">
-        <v>177</v>
+        <v>336</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="D67" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="E67" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>335</v>
+        <v>182</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C68" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="D68" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="E68" t="s">
-        <v>336</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B69" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="D69" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
       <c r="E69" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B70" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="D70" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
       <c r="E70" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C71" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="D71" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="E71" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C72" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="D72" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="E72" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B73" t="s">
         <v>38</v>
       </c>
       <c r="C73" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="D73" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="E73" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B74" t="s">
         <v>38</v>
       </c>
       <c r="C74" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="D74" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="E74" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B75" t="s">
         <v>38</v>
       </c>
       <c r="C75" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D75" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E75" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B76" t="s">
         <v>38</v>
       </c>
       <c r="C76" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D76" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E76" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B77" t="s">
         <v>38</v>
@@ -2706,15 +2713,15 @@
         <v>107</v>
       </c>
       <c r="D77" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="E77" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B78" t="s">
         <v>38</v>
@@ -2723,15 +2730,15 @@
         <v>107</v>
       </c>
       <c r="D78" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="E78" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B79" t="s">
         <v>38</v>
@@ -2740,15 +2747,15 @@
         <v>107</v>
       </c>
       <c r="D79" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E79" t="s">
-        <v>203</v>
+        <v>334</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B80" t="s">
         <v>38</v>
@@ -2757,219 +2764,219 @@
         <v>107</v>
       </c>
       <c r="D80" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E80" t="s">
-        <v>205</v>
+        <v>333</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B81" t="s">
         <v>38</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="D81" t="s">
-        <v>207</v>
+        <v>58</v>
       </c>
       <c r="E81" t="s">
-        <v>334</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B82" t="s">
         <v>38</v>
       </c>
       <c r="C82" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="D82" t="s">
-        <v>207</v>
+        <v>58</v>
       </c>
       <c r="E82" t="s">
-        <v>333</v>
+        <v>212</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B83" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="D83" t="s">
-        <v>58</v>
+        <v>214</v>
       </c>
       <c r="E83" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="B84" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="D84" t="s">
-        <v>58</v>
+        <v>214</v>
       </c>
       <c r="E84" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C85" t="s">
-        <v>27</v>
+        <v>120</v>
       </c>
       <c r="D85" t="s">
-        <v>214</v>
+        <v>121</v>
       </c>
       <c r="E85" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B86" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C86" t="s">
-        <v>27</v>
+        <v>120</v>
       </c>
       <c r="D86" t="s">
-        <v>214</v>
+        <v>121</v>
       </c>
       <c r="E86" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B87" t="s">
         <v>63</v>
       </c>
       <c r="C87" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D87" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E87" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B88" t="s">
         <v>63</v>
       </c>
       <c r="C88" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D88" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E88" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B89" t="s">
         <v>63</v>
       </c>
       <c r="C89" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D89" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E89" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B90" t="s">
         <v>63</v>
       </c>
       <c r="C90" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D90" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E90" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B91" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C91" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="D91" t="s">
-        <v>129</v>
+        <v>231</v>
       </c>
       <c r="E91" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B92" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C92" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="D92" t="s">
-        <v>129</v>
+        <v>231</v>
       </c>
       <c r="E92" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B93" t="s">
         <v>38</v>
@@ -2978,15 +2985,15 @@
         <v>39</v>
       </c>
       <c r="D93" t="s">
-        <v>231</v>
+        <v>40</v>
       </c>
       <c r="E93" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B94" t="s">
         <v>38</v>
@@ -2995,185 +3002,185 @@
         <v>39</v>
       </c>
       <c r="D94" t="s">
-        <v>231</v>
+        <v>40</v>
       </c>
       <c r="E94" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B95" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C95" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D95" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E95" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B96" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C96" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D96" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E96" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B97" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C97" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D97" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E97" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B98" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C98" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D98" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E98" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B99" t="s">
         <v>38</v>
       </c>
       <c r="C99" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D99" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E99" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B100" t="s">
         <v>38</v>
       </c>
       <c r="C100" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D100" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E100" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B101" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C101" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D101" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E101" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B102" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C102" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D102" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E102" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B103" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C103" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="D103" t="s">
-        <v>47</v>
+        <v>202</v>
       </c>
       <c r="E103" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B104" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C104" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="D104" t="s">
-        <v>47</v>
+        <v>202</v>
       </c>
       <c r="E104" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B105" t="s">
         <v>38</v>
@@ -3182,15 +3189,15 @@
         <v>107</v>
       </c>
       <c r="D105" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E105" t="s">
-        <v>256</v>
+        <v>337</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B106" t="s">
         <v>38</v>
@@ -3199,15 +3206,15 @@
         <v>107</v>
       </c>
       <c r="D106" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E106" t="s">
-        <v>258</v>
+        <v>338</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>259</v>
+        <v>208</v>
       </c>
       <c r="B107" t="s">
         <v>38</v>
@@ -3219,12 +3226,12 @@
         <v>207</v>
       </c>
       <c r="E107" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>260</v>
+        <v>206</v>
       </c>
       <c r="B108" t="s">
         <v>38</v>
@@ -3236,7 +3243,7 @@
         <v>207</v>
       </c>
       <c r="E108" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>